<commit_message>
điểm của từng nhóm
</commit_message>
<xml_diff>
--- a/CHAM_DIEM_CS112.xlsx
+++ b/CHAM_DIEM_CS112.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htpho\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD688D8-1738-42C9-A3A9-C62C6ACEAD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2566237B-41A9-4057-8D90-E1A0303770E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36EA15F2-7B79-4542-B86D-91A3EEAF9C83}"/>
   </bookViews>
@@ -168,19 +168,19 @@
     <t>Nhóm tích cực tìm hiểu, nhóm nộp đầu tiên</t>
   </si>
   <si>
-    <t>Thuật toán đếm tỉ lệ 36 sáng tạo</t>
-  </si>
-  <si>
     <t>Có đi tìm nhanh vùng 36</t>
   </si>
   <si>
     <t>Nhóm code đẹp, trực quan, thuật toán hướng tâm khá lạ</t>
   </si>
   <si>
-    <t>liems</t>
-  </si>
-  <si>
     <t>thuật convex hull lạ</t>
+  </si>
+  <si>
+    <t>Nhóm tích cực làm bài</t>
+  </si>
+  <si>
+    <t>Thuật toán tính tỉ lệ 36 mới mẻ</t>
   </si>
 </sst>
 </file>
@@ -470,9 +470,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -516,7 +515,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -528,9 +526,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -556,6 +551,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,7 +891,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,489 +905,491 @@
     <col min="7" max="7" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="30.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="12">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="11">
         <v>1</v>
       </c>
-      <c r="E1" s="12">
+      <c r="E1" s="11">
         <v>4</v>
       </c>
-      <c r="F1" s="12">
+      <c r="F1" s="11">
         <v>3</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="11">
         <v>1</v>
       </c>
-      <c r="H1" s="12">
+      <c r="H1" s="11">
         <v>1</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="11">
         <v>2</v>
       </c>
-      <c r="J1" s="15"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="30" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="14"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="13">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>2</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="14">
+      <c r="D4" s="22"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>3</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="28" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>4</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>5</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>6</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>7</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>8</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>9</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>10</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>11</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>12</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>13</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>14</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>15</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>17</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
-        <v>4</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
-        <v>5</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
-        <v>6</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>7</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
-        <v>8</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
-        <v>9</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
-        <v>10</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
-        <v>11</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
-        <v>12</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
-        <v>13</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
-        <v>14</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
-        <v>15</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="24" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
-        <v>17</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="J18" s="14">
-        <v>10</v>
+      <c r="J18" s="13">
+        <v>9.5</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="24" x14ac:dyDescent="0.4">
-      <c r="E21" s="16"/>
-      <c r="F21" s="17">
+      <c r="E21" s="15"/>
+      <c r="F21" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="24" x14ac:dyDescent="0.4">
-      <c r="E22" s="18"/>
-      <c r="F22" s="17">
+      <c r="E22" s="17"/>
+      <c r="F22" s="16">
         <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.4">
-      <c r="E23" s="26"/>
-      <c r="F23" s="17">
+      <c r="E23" s="24"/>
+      <c r="F23" s="16">
         <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E24" s="19"/>
-      <c r="F24" s="17">
+      <c r="E24" s="18"/>
+      <c r="F24" s="16">
         <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="24" x14ac:dyDescent="0.4">
-      <c r="E25" s="4"/>
-      <c r="F25" s="17">
+      <c r="E25" s="3"/>
+      <c r="F25" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="5"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="5"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="5"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F29" s="5"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="5"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="5"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F32" s="5"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="5"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="5"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="5"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="5"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="5"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="5"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="5"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="5"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F41" s="5"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F42" s="5"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F43" s="5"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="5"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="5"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="5"/>
+      <c r="F46" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1413,187 +1413,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6">
+      <c r="A1" s="5">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>10</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>11</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <v>12</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>13</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>14</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>15</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <v>16</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>17</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cập nhật điểm và tiêu chí
</commit_message>
<xml_diff>
--- a/CHAM_DIEM_CS112.xlsx
+++ b/CHAM_DIEM_CS112.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htpho\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htpho\OneDrive\Documents\GitHub\CS112_BruteForce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2566237B-41A9-4057-8D90-E1A0303770E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41402BC7-432A-47D7-A47E-DB49544DAE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36EA15F2-7B79-4542-B86D-91A3EEAF9C83}"/>
   </bookViews>
@@ -162,9 +162,6 @@
     <t>Tổng (MAX = 10)</t>
   </si>
   <si>
-    <t>Nhóm tích cực tìm hiểu</t>
-  </si>
-  <si>
     <t>Nhóm tích cực tìm hiểu, nhóm nộp đầu tiên</t>
   </si>
   <si>
@@ -177,10 +174,13 @@
     <t>thuật convex hull lạ</t>
   </si>
   <si>
-    <t>Nhóm tích cực làm bài</t>
-  </si>
-  <si>
     <t>Thuật toán tính tỉ lệ 36 mới mẻ</t>
+  </si>
+  <si>
+    <t>Nhóm tích cực tìm hiểu, nhóm nộp sớm</t>
+  </si>
+  <si>
+    <t>Nhóm tích cực làm bài + code OOP đẹp</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -521,9 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -891,7 +888,7 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,19 +912,19 @@
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="11">
         <v>4</v>
       </c>
       <c r="F1" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G1" s="11">
         <v>1</v>
       </c>
       <c r="H1" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I1" s="11">
         <v>2</v>
@@ -938,24 +935,24 @@
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="12" t="s">
@@ -966,16 +963,16 @@
       <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="22"/>
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="33"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="13">
         <v>9</v>
       </c>
@@ -984,10 +981,10 @@
       <c r="A4" s="21">
         <v>2</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="22"/>
@@ -995,7 +992,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="34"/>
+      <c r="I4" s="33"/>
       <c r="J4" s="13">
         <v>9</v>
       </c>
@@ -1004,32 +1001,32 @@
       <c r="A5" s="21">
         <v>3</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="22"/>
-      <c r="E5" s="35"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="26" t="s">
-        <v>45</v>
+      <c r="I5" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="J5" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>4</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="22"/>
@@ -1037,21 +1034,21 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="25" t="s">
-        <v>46</v>
+      <c r="I6" s="35" t="s">
+        <v>47</v>
       </c>
       <c r="J6" s="13">
-        <v>10</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>5</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="22"/>
@@ -1059,19 +1056,19 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="33"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="13">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>6</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="22"/>
@@ -1080,7 +1077,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="25" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J8" s="13">
         <v>10</v>
@@ -1090,10 +1087,10 @@
       <c r="A9" s="21">
         <v>7</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="22"/>
@@ -1101,7 +1098,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="33"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="13">
         <v>9</v>
       </c>
@@ -1110,10 +1107,10 @@
       <c r="A10" s="21">
         <v>8</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="22"/>
@@ -1121,7 +1118,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="33"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="13">
         <v>9</v>
       </c>
@@ -1130,10 +1127,10 @@
       <c r="A11" s="21">
         <v>9</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="22"/>
@@ -1141,8 +1138,8 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="26" t="s">
-        <v>44</v>
+      <c r="I11" s="25" t="s">
+        <v>43</v>
       </c>
       <c r="J11" s="13">
         <v>10</v>
@@ -1152,10 +1149,10 @@
       <c r="A12" s="21">
         <v>10</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="22"/>
@@ -1163,7 +1160,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="33"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="13">
         <v>9</v>
       </c>
@@ -1172,10 +1169,10 @@
       <c r="A13" s="21">
         <v>11</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="22"/>
@@ -1183,8 +1180,8 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="26" t="s">
-        <v>42</v>
+      <c r="I13" s="25" t="s">
+        <v>41</v>
       </c>
       <c r="J13" s="13">
         <v>10</v>
@@ -1194,10 +1191,10 @@
       <c r="A14" s="21">
         <v>12</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="22"/>
@@ -1205,7 +1202,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="33"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="13">
         <v>10</v>
       </c>
@@ -1214,10 +1211,10 @@
       <c r="A15" s="21">
         <v>13</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="22"/>
@@ -1225,7 +1222,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="33"/>
+      <c r="I15" s="32"/>
       <c r="J15" s="13">
         <v>9</v>
       </c>
@@ -1234,10 +1231,10 @@
       <c r="A16" s="21">
         <v>14</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="22"/>
@@ -1245,7 +1242,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="33"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="13">
         <v>9</v>
       </c>
@@ -1254,10 +1251,10 @@
       <c r="A17" s="21">
         <v>15</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="30" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="22"/>
@@ -1265,7 +1262,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="33"/>
+      <c r="I17" s="32"/>
       <c r="J17" s="13">
         <v>9</v>
       </c>
@@ -1274,10 +1271,10 @@
       <c r="A18" s="21">
         <v>17</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="22"/>
@@ -1285,8 +1282,8 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="36" t="s">
-        <v>47</v>
+      <c r="I18" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="J18" s="13">
         <v>9.5</v>
@@ -1783,20 +1780,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7804a6fb-3003-4c78-85cc-87186ae6e246" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7804a6fb-3003-4c78-85cc-87186ae6e246" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1818,14 +1815,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84A0474E-4514-4B87-B512-D66C38D68954}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9B23C76-F988-43EE-A49B-A4CEB9D14081}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1839,4 +1828,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84A0474E-4514-4B87-B512-D66C38D68954}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>